<commit_message>
update mattermost seeder, excel, tenant
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,18 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minh/Project/Multi-tenant/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB3C2B6-DAB6-0745-B8F2-E48C1C7FC48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="17380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Classes" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Users" sheetId="2" r:id="rId5"/>
+    <sheet name="Classes" sheetId="1" r:id="rId1"/>
+    <sheet name="Subjects" sheetId="2" r:id="rId2"/>
+    <sheet name="Users" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>code</t>
   </si>
@@ -29,7 +39,7 @@
     <t>Lớp 10A1</t>
   </si>
   <si>
-    <t>Lớp chọn Toán - GVCN: Nguyễn Văn Toán</t>
+    <t>Lớp Chọn Toán</t>
   </si>
   <si>
     <t>11B2</t>
@@ -38,16 +48,61 @@
     <t>Lớp 11B2</t>
   </si>
   <si>
-    <t>Lớp xã hội - GVCN: Lê Thị Văn</t>
-  </si>
-  <si>
-    <t>12C1</t>
-  </si>
-  <si>
-    <t>Lớp 12C1</t>
-  </si>
-  <si>
-    <t>Lớp định hướng CNTT</t>
+    <t>Lớp Xã Hội</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>Môn Toán</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Thảo luận môn Toán</t>
+  </si>
+  <si>
+    <t>LIT</t>
+  </si>
+  <si>
+    <t>Môn Văn</t>
+  </si>
+  <si>
+    <t>Thảo luận môn Văn</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>Tiếng Anh</t>
+  </si>
+  <si>
+    <t>Thảo luận Tiếng Anh</t>
+  </si>
+  <si>
+    <t>PARENTS</t>
+  </si>
+  <si>
+    <t>Phụ Huynh</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Kênh kín cho PH</t>
+  </si>
+  <si>
+    <t>TEACHERS</t>
+  </si>
+  <si>
+    <t>Giáo Viên</t>
+  </si>
+  <si>
+    <t>Kênh kín nội bộ GV</t>
   </si>
   <si>
     <t>email</t>
@@ -68,76 +123,79 @@
     <t>class_code</t>
   </si>
   <si>
-    <t>gv_toan@school.edu</t>
-  </si>
-  <si>
-    <t>gv_toan</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Toán</t>
+    <t>gv_toan@truong.edu</t>
+  </si>
+  <si>
+    <t>Admin@123</t>
+  </si>
+  <si>
+    <t>Thầy Toán</t>
   </si>
   <si>
     <t>teacher</t>
   </si>
   <si>
-    <t>hs_an@school.edu</t>
-  </si>
-  <si>
-    <t>hs_an</t>
-  </si>
-  <si>
-    <t>Trần Bình An</t>
+    <t>hs_an@truong.edu</t>
+  </si>
+  <si>
+    <t>Student@123</t>
+  </si>
+  <si>
+    <t>Em An</t>
   </si>
   <si>
     <t>student</t>
   </si>
   <si>
-    <t>hs_binh@school.edu</t>
-  </si>
-  <si>
-    <t>hs_binh</t>
-  </si>
-  <si>
-    <t>Lê Thái Bình</t>
-  </si>
-  <si>
-    <t>gv_van@school.edu</t>
-  </si>
-  <si>
-    <t>gv_van</t>
-  </si>
-  <si>
-    <t>Lê Thị Văn</t>
-  </si>
-  <si>
-    <t>hs_cuong@school.edu</t>
-  </si>
-  <si>
-    <t>hs_cuong</t>
-  </si>
-  <si>
-    <t>Phạm Văn Cường</t>
+    <t>ph_an@gmail.com</t>
+  </si>
+  <si>
+    <t>Parent@123</t>
+  </si>
+  <si>
+    <t>Bố em An</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>gv-toan</t>
+  </si>
+  <si>
+    <t>hs-an</t>
+  </si>
+  <si>
+    <t>ph-an</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Google Sans Text&quot;"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Google Sans Text&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,43 +203,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -371,20 +431,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -395,7 +458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -406,7 +469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -417,153 +480,230 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1">
-        <v>123456.0</v>
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1">
-        <v>123456.0</v>
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1">
-        <v>123456.0</v>
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1">
-        <v>123456.0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1">
-        <v>123456.0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>